<commit_message>
Bunch of Changes for UDF Network issues
</commit_message>
<xml_diff>
--- a/vegakub/IP Plan/Book1.xlsx
+++ b/vegakub/IP Plan/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grimard/Documents/GitHub/vagrant/vegakub/IP Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525E8148-9D8F-A647-929A-75E6331EB224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB1F7F3-1447-F149-9EC7-1B084A73214D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44340" yWindow="4100" windowWidth="60160" windowHeight="28340" xr2:uid="{E9FCD930-FFAC-164A-8BF6-52448EE179D8}"/>
+    <workbookView minimized="1" xWindow="-60160" yWindow="460" windowWidth="60160" windowHeight="28340" xr2:uid="{E9FCD930-FFAC-164A-8BF6-52448EE179D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -629,7 +629,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>